<commit_message>
change the path of swf
</commit_message>
<xml_diff>
--- a/working/工作日志.杨炜.6月份.xlsx
+++ b/working/工作日志.杨炜.6月份.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28710" windowHeight="13050" activeTab="1"/>
+    <workbookView windowWidth="28710" windowHeight="13050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="第一周" sheetId="1" r:id="rId1"/>
     <sheet name="第二周" sheetId="2" r:id="rId2"/>
-    <sheet name="模板" sheetId="3" r:id="rId3"/>
+    <sheet name="第三周" sheetId="3" r:id="rId3"/>
+    <sheet name="模板" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85">
   <si>
     <t>2日工作日志（周二）</t>
   </si>
@@ -231,6 +232,58 @@
   </si>
   <si>
     <t>12日工作计划（周五）</t>
+  </si>
+  <si>
+    <t>活动结束时间改成12</t>
+  </si>
+  <si>
+    <t>首页banner√
+首页小banner√
+活动页banner√
+活动页规则√
+EDM邮件上广告√</t>
+  </si>
+  <si>
+    <t>12日工作日志（周五）</t>
+  </si>
+  <si>
+    <t>14日工作计划（周日）</t>
+  </si>
+  <si>
+    <t>制作圆形进度条的 Css Sprite</t>
+  </si>
+  <si>
+    <t>添加index hack</t>
+  </si>
+  <si>
+    <t>解决按钮显示兼容问题</t>
+  </si>
+  <si>
+    <t>制作按钮 Css Sprite</t>
+  </si>
+  <si>
+    <t>产品页面IE8下表格宽度兼容问题</t>
+  </si>
+  <si>
+    <t>14日工作日志（周日）</t>
+  </si>
+  <si>
+    <t>15日工作计划（周一）</t>
+  </si>
+  <si>
+    <t>投资列表按钮文字：
+“马上投资”改成“立即理财”
+“查看详情”改成“募集结束”</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 首页 html 文件 183 行，{$data.text}
+ 修改地方包含首页列表+产品列表页面</t>
+  </si>
+  <si>
+    <t>15日工作日志（周一）</t>
+  </si>
+  <si>
+    <t>16日工作计划（周二）</t>
   </si>
   <si>
     <t>日工作日志（周）</t>
@@ -244,10 +297,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -778,7 +831,7 @@
   <sheetPr/>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
@@ -1791,10 +1844,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2616,13 +2669,19 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" ht="16.5" spans="1:7">
+    <row r="54" ht="82.5" spans="1:7">
       <c r="A54" s="6">
         <v>4</v>
       </c>
-      <c r="B54" s="10"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
+      <c r="B54" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>69</v>
+      </c>
       <c r="E54" s="9"/>
       <c r="F54" s="6">
         <v>4</v>
@@ -2744,8 +2803,480 @@
       <c r="F63" s="13"/>
       <c r="G63" s="12"/>
     </row>
+    <row r="65" ht="18" spans="1:7">
+      <c r="A65" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G65" s="1"/>
+    </row>
+    <row r="66" ht="21" spans="1:7">
+      <c r="A66" s="3"/>
+      <c r="B66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="4"/>
+      <c r="F66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G66" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" ht="16.5" spans="1:7">
+      <c r="A67" s="6">
+        <v>1</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D67" s="7"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="6">
+        <v>1</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" ht="66" spans="1:7">
+      <c r="A68" s="6">
+        <v>2</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="6">
+        <v>2</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" ht="16.5" spans="1:7">
+      <c r="A69" s="6">
+        <v>3</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="6">
+        <v>3</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="70" ht="16.5" spans="1:7">
+      <c r="A70" s="6">
+        <v>4</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="6">
+        <v>4</v>
+      </c>
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" ht="16.5" spans="1:7">
+      <c r="A71" s="6">
+        <v>5</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="10"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="6">
+        <v>5</v>
+      </c>
+      <c r="G71" s="7"/>
+    </row>
+    <row r="72" ht="16.5" spans="1:7">
+      <c r="A72" s="6">
+        <v>6</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="6">
+        <v>6</v>
+      </c>
+      <c r="G72" s="7"/>
+    </row>
+    <row r="73" ht="16.5" spans="1:7">
+      <c r="A73" s="6">
+        <v>7</v>
+      </c>
+      <c r="B73" s="10"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="6">
+        <v>7</v>
+      </c>
+      <c r="G73" s="7"/>
+    </row>
+    <row r="74" ht="16.5" spans="1:7">
+      <c r="A74" s="6">
+        <v>8</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="6">
+        <v>8</v>
+      </c>
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" ht="16.5" spans="1:7">
+      <c r="A75" s="6">
+        <v>9</v>
+      </c>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="6">
+        <v>9</v>
+      </c>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" ht="16.5" spans="1:7">
+      <c r="A76" s="6">
+        <v>10</v>
+      </c>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="6">
+        <v>10</v>
+      </c>
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" ht="16.5" spans="1:7">
+      <c r="A77" s="6">
+        <v>11</v>
+      </c>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="6">
+        <v>11</v>
+      </c>
+      <c r="G77" s="7"/>
+    </row>
+    <row r="78" ht="16.5" spans="1:7">
+      <c r="A78" s="6">
+        <v>12</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="6">
+        <v>12</v>
+      </c>
+      <c r="G78" s="7"/>
+    </row>
+    <row r="79" ht="16.5" spans="1:7">
+      <c r="A79" s="11"/>
+      <c r="B79" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C79" s="12"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="12"/>
+    </row>
+    <row r="81" ht="18" spans="1:7">
+      <c r="A81" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" ht="21" spans="1:7">
+      <c r="A82" s="3"/>
+      <c r="B82" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="4"/>
+      <c r="F82" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" ht="16.5" spans="1:7">
+      <c r="A83" s="6">
+        <v>1</v>
+      </c>
+      <c r="B83" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="6">
+        <v>1</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" ht="66" spans="1:7">
+      <c r="A84" s="6">
+        <v>2</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E84" s="9"/>
+      <c r="F84" s="6">
+        <v>2</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" ht="16.5" spans="1:7">
+      <c r="A85" s="6">
+        <v>3</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="6">
+        <v>3</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" ht="16.5" spans="1:7">
+      <c r="A86" s="6">
+        <v>4</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D86" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E86" s="9"/>
+      <c r="F86" s="6">
+        <v>4</v>
+      </c>
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87" ht="16.5" spans="1:7">
+      <c r="A87" s="6">
+        <v>5</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D87" s="10"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="6">
+        <v>5</v>
+      </c>
+      <c r="G87" s="7"/>
+    </row>
+    <row r="88" ht="16.5" spans="1:7">
+      <c r="A88" s="6">
+        <v>6</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D88" s="7"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="6">
+        <v>6</v>
+      </c>
+      <c r="G88" s="7"/>
+    </row>
+    <row r="89" ht="49.5" spans="1:7">
+      <c r="A89" s="6">
+        <v>7</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E89" s="9"/>
+      <c r="F89" s="6">
+        <v>7</v>
+      </c>
+      <c r="G89" s="7"/>
+    </row>
+    <row r="90" ht="16.5" spans="1:7">
+      <c r="A90" s="6">
+        <v>8</v>
+      </c>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="6">
+        <v>8</v>
+      </c>
+      <c r="G90" s="7"/>
+    </row>
+    <row r="91" ht="16.5" spans="1:7">
+      <c r="A91" s="6">
+        <v>9</v>
+      </c>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="6">
+        <v>9</v>
+      </c>
+      <c r="G91" s="7"/>
+    </row>
+    <row r="92" ht="16.5" spans="1:7">
+      <c r="A92" s="6">
+        <v>10</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="6">
+        <v>10</v>
+      </c>
+      <c r="G92" s="7"/>
+    </row>
+    <row r="93" ht="16.5" spans="1:7">
+      <c r="A93" s="6">
+        <v>11</v>
+      </c>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="6">
+        <v>11</v>
+      </c>
+      <c r="G93" s="7"/>
+    </row>
+    <row r="94" ht="16.5" spans="1:7">
+      <c r="A94" s="6">
+        <v>12</v>
+      </c>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="6">
+        <v>12</v>
+      </c>
+      <c r="G94" s="7"/>
+    </row>
+    <row r="95" ht="16.5" spans="1:7">
+      <c r="A95" s="11"/>
+      <c r="B95" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
+      <c r="E95" s="12"/>
+      <c r="F95" s="13"/>
+      <c r="G95" s="12"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="24">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="B15:G15"/>
@@ -2758,10 +3289,18 @@
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="B63:G63"/>
+    <mergeCell ref="A65:D65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="B79:G79"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="B95:G95"/>
     <mergeCell ref="E3:E14"/>
     <mergeCell ref="E19:E30"/>
     <mergeCell ref="E35:E46"/>
     <mergeCell ref="E51:E62"/>
+    <mergeCell ref="E67:E78"/>
+    <mergeCell ref="E83:E94"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -2770,6 +3309,277 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="7.125" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="34.875" customWidth="1"/>
+    <col min="4" max="4" width="33.25" customWidth="1"/>
+    <col min="5" max="5" width="6.75" customWidth="1"/>
+    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="7" max="7" width="35.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" ht="21" spans="1:7">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" ht="16.5" spans="1:7">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" ht="66" spans="1:7">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="16.5" spans="1:7">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="16.5" spans="1:7">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" ht="16.5" spans="1:7">
+      <c r="A7" s="6">
+        <v>5</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="6">
+        <v>5</v>
+      </c>
+      <c r="G7" s="7"/>
+    </row>
+    <row r="8" ht="16.5" spans="1:7">
+      <c r="A8" s="6">
+        <v>6</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="6">
+        <v>6</v>
+      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9" ht="16.5" spans="1:7">
+      <c r="A9" s="6">
+        <v>7</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="6">
+        <v>7</v>
+      </c>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" ht="16.5" spans="1:7">
+      <c r="A10" s="6">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="6">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" ht="16.5" spans="1:7">
+      <c r="A11" s="6">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="6">
+        <v>9</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" ht="16.5" spans="1:7">
+      <c r="A12" s="6">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="6">
+        <v>10</v>
+      </c>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" ht="16.5" spans="1:7">
+      <c r="A13" s="6">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="6">
+        <v>11</v>
+      </c>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" ht="16.5" spans="1:7">
+      <c r="A14" s="6">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="6">
+        <v>12</v>
+      </c>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" ht="16.5" spans="1:7">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="3:3">
+      <c r="C16">
+        <v>9999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="E3:E14"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
   <dimension ref="A1:G15"/>
@@ -2791,14 +3601,14 @@
   <sheetData>
     <row r="1" ht="18" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
       <c r="F1" s="1" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="G1" s="1"/>
     </row>

</xml_diff>